<commit_message>
added borrowerPairs Utils, updated encompass
</commit_message>
<xml_diff>
--- a/test_Data/NewLoan.xlsx
+++ b/test_Data/NewLoan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NagaSaiSriharshaKara\Desktop\PRMG\test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED71399E-6E98-4BA0-A634-299CB90FEAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD79457-A102-474A-84F4-F7A2721DB522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{C1C90F5A-236F-411C-9C72-6F452735E766}"/>
   </bookViews>
@@ -1304,11 +1304,11 @@
   <dimension ref="A1:CM527"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Y2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AY2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E19" sqref="E19"/>
       <selection pane="topRight" activeCell="E19" sqref="E19"/>
       <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
-      <selection pane="bottomRight" activeCell="AH5" sqref="AH5"/>
+      <selection pane="bottomRight" activeCell="BI7" sqref="BI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18993,6 +18993,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="f55b03ab-a17e-45ae-bce8-30e2886d64f3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010036886560AE7D0346A967BB2F04832EDE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1847e798d1e94f2c11a530a0a74dc730">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f55b03ab-a17e-45ae-bce8-30e2886d64f3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc1af3afbe156bc2be057a66c6dbf5dc" ns3:_="">
     <xsd:import namespace="f55b03ab-a17e-45ae-bce8-30e2886d64f3"/>
@@ -19174,24 +19191,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49BEC817-B763-4B8D-BE16-B76A4BBC14A4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="f55b03ab-a17e-45ae-bce8-30e2886d64f3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="f55b03ab-a17e-45ae-bce8-30e2886d64f3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2688610-0CFD-4DBB-91CE-6FA05FF6834E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABE8BC61-4CF1-4FE5-A634-CDA60DE3AD74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19207,28 +19231,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2688610-0CFD-4DBB-91CE-6FA05FF6834E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49BEC817-B763-4B8D-BE16-B76A4BBC14A4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="f55b03ab-a17e-45ae-bce8-30e2886d64f3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>